<commit_message>
Fix label angle in plot axes
</commit_message>
<xml_diff>
--- a/TN042/foldchange_dox.xlsx
+++ b/TN042/foldchange_dox.xlsx
@@ -451,7 +451,7 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>dusp11 foldchange</t>
+          <t xml:space="preserve">dusp11 </t>
         </is>
       </c>
       <c r="C2" t="n">
@@ -464,7 +464,7 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>ifnb foldchange</t>
+          <t xml:space="preserve">ifnb </t>
         </is>
       </c>
       <c r="C3" t="n">
@@ -477,7 +477,7 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>mx1 foldchange</t>
+          <t xml:space="preserve">mx1 </t>
         </is>
       </c>
       <c r="C4" t="n">

</xml_diff>